<commit_message>
Added comments to analysis run file
</commit_message>
<xml_diff>
--- a/data/MTF_database.xlsx
+++ b/data/MTF_database.xlsx
@@ -11508,7 +11508,7 @@
         <v>-120.369965</v>
       </c>
       <c r="I8">
-        <v>22.97748209326372</v>
+        <v>22.99612514168063</v>
       </c>
       <c r="J8" t="s">
         <v>221</v>
@@ -11648,7 +11648,7 @@
         <v>-120.369965</v>
       </c>
       <c r="I9">
-        <v>45.96982103826346</v>
+        <v>46.04826764372285</v>
       </c>
       <c r="J9" t="s">
         <v>221</v>
@@ -14698,7 +14698,7 @@
         <v>-115</v>
       </c>
       <c r="I31">
-        <v>18.10980502209353</v>
+        <v>18.10991498197173</v>
       </c>
       <c r="J31" t="s">
         <v>233</v>
@@ -14732,9 +14732,6 @@
       </c>
       <c r="U31">
         <v>18.20130399348003</v>
-      </c>
-      <c r="V31">
-        <v>1</v>
       </c>
       <c r="W31">
         <v>1</v>
@@ -14835,7 +14832,7 @@
         <v>-115</v>
       </c>
       <c r="I32">
-        <v>18.34124274544953</v>
+        <v>18.3412519881067</v>
       </c>
       <c r="J32" t="s">
         <v>233</v>
@@ -14869,9 +14866,6 @@
       </c>
       <c r="U32">
         <v>18.20130399348003</v>
-      </c>
-      <c r="V32">
-        <v>1</v>
       </c>
       <c r="W32">
         <v>1</v>
@@ -15520,7 +15514,7 @@
         <v>89</v>
       </c>
       <c r="I37">
-        <v>22.89891898833984</v>
+        <v>22.92306133575505</v>
       </c>
       <c r="J37" t="s">
         <v>236</v>
@@ -15573,7 +15567,7 @@
         <v>89</v>
       </c>
       <c r="I38">
-        <v>44.56587613510701</v>
+        <v>44.61286197164648</v>
       </c>
       <c r="J38" t="s">
         <v>236</v>
@@ -15635,7 +15629,7 @@
         <v>-79.5</v>
       </c>
       <c r="I39">
-        <v>8.007011828479676</v>
+        <v>8.063352523741193</v>
       </c>
       <c r="J39" t="s">
         <v>227</v>
@@ -15775,7 +15769,7 @@
         <v>-79.5</v>
       </c>
       <c r="I40">
-        <v>11.01763582135013</v>
+        <v>11.06617244552393</v>
       </c>
       <c r="J40" t="s">
         <v>227</v>
@@ -15947,9 +15941,6 @@
       <c r="U41">
         <v>27.8859865470852</v>
       </c>
-      <c r="V41">
-        <v>1</v>
-      </c>
       <c r="W41">
         <v>1</v>
       </c>
@@ -16084,9 +16075,6 @@
       <c r="U42">
         <v>27.8859865470852</v>
       </c>
-      <c r="V42">
-        <v>1</v>
-      </c>
       <c r="W42">
         <v>1</v>
       </c>
@@ -16186,7 +16174,7 @@
         <v>-94.25</v>
       </c>
       <c r="I43">
-        <v>6.650027499973381</v>
+        <v>6.676535156145438</v>
       </c>
       <c r="J43" t="s">
         <v>222</v>
@@ -16314,7 +16302,7 @@
         <v>-94.25</v>
       </c>
       <c r="I44">
-        <v>12.9422835204482</v>
+        <v>12.99387272089025</v>
       </c>
       <c r="J44" t="s">
         <v>222</v>
@@ -16891,9 +16879,6 @@
       <c r="U48">
         <v>14</v>
       </c>
-      <c r="V48">
-        <v>1</v>
-      </c>
       <c r="W48">
         <v>1</v>
       </c>
@@ -17028,9 +17013,6 @@
       <c r="U49">
         <v>14</v>
       </c>
-      <c r="V49">
-        <v>1</v>
-      </c>
       <c r="W49">
         <v>1</v>
       </c>
@@ -22093,7 +22075,7 @@
         <v>-118.563032</v>
       </c>
       <c r="I88">
-        <v>7.301056893307665</v>
+        <v>7.301968965493928</v>
       </c>
       <c r="J88" t="s">
         <v>219</v>
@@ -22236,7 +22218,7 @@
         <v>-118.563032</v>
       </c>
       <c r="I89">
-        <v>8.007077228112996</v>
+        <v>8.006009769663372</v>
       </c>
       <c r="J89" t="s">
         <v>219</v>
@@ -27010,9 +26992,6 @@
       <c r="U132">
         <v>10.35282258064516</v>
       </c>
-      <c r="V132">
-        <v>1</v>
-      </c>
       <c r="W132">
         <v>1</v>
       </c>
@@ -27150,9 +27129,6 @@
       <c r="U133">
         <v>10.35282258064516</v>
       </c>
-      <c r="V133">
-        <v>1</v>
-      </c>
       <c r="W133">
         <v>1</v>
       </c>
@@ -27683,9 +27659,6 @@
       <c r="U137">
         <v>54.44464609800364</v>
       </c>
-      <c r="V137">
-        <v>1</v>
-      </c>
       <c r="W137">
         <v>1</v>
       </c>
@@ -27823,9 +27796,6 @@
       <c r="U138">
         <v>54.44464609800364</v>
       </c>
-      <c r="V138">
-        <v>1</v>
-      </c>
       <c r="W138">
         <v>1</v>
       </c>
@@ -33566,9 +33536,6 @@
       <c r="T179" t="b">
         <v>0</v>
       </c>
-      <c r="V179">
-        <v>1</v>
-      </c>
       <c r="W179">
         <v>1</v>
       </c>
@@ -33700,9 +33667,6 @@
       <c r="T180" t="b">
         <v>0</v>
       </c>
-      <c r="V180">
-        <v>1</v>
-      </c>
       <c r="W180">
         <v>1</v>
       </c>
@@ -36577,9 +36541,6 @@
       <c r="T201" t="b">
         <v>0</v>
       </c>
-      <c r="V201">
-        <v>1</v>
-      </c>
       <c r="X201">
         <v>0</v>
       </c>
@@ -36621,9 +36582,6 @@
       <c r="T202" t="b">
         <v>0</v>
       </c>
-      <c r="V202">
-        <v>1</v>
-      </c>
       <c r="X202">
         <v>0</v>
       </c>
@@ -36692,9 +36650,6 @@
       <c r="T203" t="b">
         <v>0</v>
       </c>
-      <c r="V203">
-        <v>1</v>
-      </c>
       <c r="W203">
         <v>0</v>
       </c>
@@ -36826,9 +36781,6 @@
       <c r="T204" t="b">
         <v>0</v>
       </c>
-      <c r="V204">
-        <v>1</v>
-      </c>
       <c r="W204">
         <v>0</v>
       </c>
@@ -37505,9 +37457,6 @@
       <c r="U209">
         <v>29.43243243243243</v>
       </c>
-      <c r="V209">
-        <v>1</v>
-      </c>
       <c r="W209">
         <v>1</v>
       </c>
@@ -37648,9 +37597,6 @@
       <c r="U210">
         <v>29.43243243243243</v>
       </c>
-      <c r="V210">
-        <v>1</v>
-      </c>
       <c r="W210">
         <v>1</v>
       </c>
@@ -38142,9 +38088,6 @@
       <c r="U217">
         <v>51.50866207472343</v>
       </c>
-      <c r="V217">
-        <v>1</v>
-      </c>
       <c r="W217">
         <v>1</v>
       </c>
@@ -38282,9 +38225,6 @@
       <c r="U218">
         <v>51.50866207472343</v>
       </c>
-      <c r="V218">
-        <v>1</v>
-      </c>
       <c r="W218">
         <v>1</v>
       </c>
@@ -38418,9 +38358,6 @@
       </c>
       <c r="T219" t="b">
         <v>0</v>
-      </c>
-      <c r="V219">
-        <v>1</v>
       </c>
       <c r="W219">
         <v>1</v>
@@ -40767,7 +40704,7 @@
         <v>-120.369965</v>
       </c>
       <c r="I11">
-        <v>21.273874865918</v>
+        <v>21.27337786011708</v>
       </c>
       <c r="J11" t="s">
         <v>489</v>
@@ -40916,7 +40853,7 @@
         <v>-120.369965</v>
       </c>
       <c r="I12">
-        <v>16.95569578534599</v>
+        <v>16.96936410255086</v>
       </c>
       <c r="J12" t="s">
         <v>490</v>
@@ -41232,7 +41169,7 @@
         <v>-120.369965</v>
       </c>
       <c r="I14">
-        <v>52.95774533497393</v>
+        <v>53.3879139090967</v>
       </c>
       <c r="J14" t="s">
         <v>491</v>
@@ -41545,7 +41482,7 @@
         <v>-120.369965</v>
       </c>
       <c r="I16">
-        <v>25.96933635382329</v>
+        <v>25.96757471699018</v>
       </c>
       <c r="J16" t="s">
         <v>489</v>
@@ -41694,7 +41631,7 @@
         <v>-120.369965</v>
       </c>
       <c r="I17">
-        <v>18.52381438887396</v>
+        <v>18.58457916945005</v>
       </c>
       <c r="J17" t="s">
         <v>490</v>
@@ -42010,7 +41947,7 @@
         <v>-120.369965</v>
       </c>
       <c r="I19">
-        <v>61.31847753716489</v>
+        <v>61.98591835576939</v>
       </c>
       <c r="J19" t="s">
         <v>491</v>
@@ -48730,7 +48667,7 @@
         <v>-115</v>
       </c>
       <c r="I61">
-        <v>18.10980502209353</v>
+        <v>18.10991498197173</v>
       </c>
       <c r="J61" t="s">
         <v>504</v>
@@ -48770,9 +48707,6 @@
       </c>
       <c r="W61">
         <v>18.20130399348003</v>
-      </c>
-      <c r="X61">
-        <v>1</v>
       </c>
       <c r="Y61">
         <v>0</v>
@@ -48891,7 +48825,7 @@
         <v>-115</v>
       </c>
       <c r="I62">
-        <v>18.34124274544953</v>
+        <v>18.3412519881067</v>
       </c>
       <c r="J62" t="s">
         <v>504</v>
@@ -48931,9 +48865,6 @@
       </c>
       <c r="W62">
         <v>18.20130399348003</v>
-      </c>
-      <c r="X62">
-        <v>1</v>
       </c>
       <c r="Y62">
         <v>0</v>
@@ -49690,7 +49621,7 @@
         <v>89</v>
       </c>
       <c r="I67">
-        <v>20.08644838508577</v>
+        <v>20.10530244052105</v>
       </c>
       <c r="J67" t="s">
         <v>505</v>
@@ -49767,7 +49698,7 @@
         <v>89</v>
       </c>
       <c r="I68">
-        <v>41.30781748236655</v>
+        <v>41.36657410455943</v>
       </c>
       <c r="J68" t="s">
         <v>506</v>
@@ -49841,7 +49772,7 @@
         <v>89</v>
       </c>
       <c r="I69">
-        <v>29.73196089960395</v>
+        <v>29.75986867245926</v>
       </c>
       <c r="J69" t="s">
         <v>505</v>
@@ -49918,7 +49849,7 @@
         <v>89</v>
       </c>
       <c r="I70">
-        <v>61.14383143739897</v>
+        <v>61.23080298956887</v>
       </c>
       <c r="J70" t="s">
         <v>506</v>
@@ -50001,7 +49932,7 @@
         <v>-79.5</v>
       </c>
       <c r="I71">
-        <v>7.926896036830874</v>
+        <v>7.989844586796213</v>
       </c>
       <c r="J71" t="s">
         <v>507</v>
@@ -50162,7 +50093,7 @@
         <v>-79.5</v>
       </c>
       <c r="I72">
-        <v>9.946843309222483</v>
+        <v>9.986135857581068</v>
       </c>
       <c r="J72" t="s">
         <v>508</v>
@@ -50323,7 +50254,7 @@
         <v>-79.5</v>
       </c>
       <c r="I73">
-        <v>7.597376725591749</v>
+        <v>7.640949391632129</v>
       </c>
       <c r="J73" t="s">
         <v>509</v>
@@ -50478,7 +50409,7 @@
         <v>-79.5</v>
       </c>
       <c r="I74">
-        <v>5.473655949659983</v>
+        <v>5.486369373339834</v>
       </c>
       <c r="J74" t="s">
         <v>510</v>
@@ -50627,7 +50558,7 @@
         <v>-79.5</v>
       </c>
       <c r="I75">
-        <v>9.426624977189752</v>
+        <v>9.466138738756532</v>
       </c>
       <c r="J75" t="s">
         <v>511</v>
@@ -50791,7 +50722,7 @@
         <v>-79.5</v>
       </c>
       <c r="I76">
-        <v>8.938738611005734</v>
+        <v>9.016132490695149</v>
       </c>
       <c r="J76" t="s">
         <v>512</v>
@@ -50946,7 +50877,7 @@
         <v>-79.5</v>
       </c>
       <c r="I77">
-        <v>10.23468914554558</v>
+        <v>10.32401558541339</v>
       </c>
       <c r="J77" t="s">
         <v>513</v>
@@ -51101,7 +51032,7 @@
         <v>-79.5</v>
       </c>
       <c r="I78">
-        <v>4.836017848215848</v>
+        <v>4.863709208897453</v>
       </c>
       <c r="J78" t="s">
         <v>514</v>
@@ -51256,7 +51187,7 @@
         <v>-79.5</v>
       </c>
       <c r="I79">
-        <v>6.857049000752933</v>
+        <v>6.889141050169556</v>
       </c>
       <c r="J79" t="s">
         <v>515</v>
@@ -51420,7 +51351,7 @@
         <v>-79.5</v>
       </c>
       <c r="I80">
-        <v>7.480496043202013</v>
+        <v>7.549580417035496</v>
       </c>
       <c r="J80" t="s">
         <v>501</v>
@@ -51584,7 +51515,7 @@
         <v>-79.5</v>
       </c>
       <c r="I81">
-        <v>7.797613947636187</v>
+        <v>7.867916947462382</v>
       </c>
       <c r="J81" t="s">
         <v>516</v>
@@ -51745,7 +51676,7 @@
         <v>-79.5</v>
       </c>
       <c r="I82">
-        <v>10.77751660060732</v>
+        <v>10.83506253449266</v>
       </c>
       <c r="J82" t="s">
         <v>507</v>
@@ -51906,7 +51837,7 @@
         <v>-79.5</v>
       </c>
       <c r="I83">
-        <v>15.06084167793178</v>
+        <v>15.07151281776448</v>
       </c>
       <c r="J83" t="s">
         <v>508</v>
@@ -52067,7 +51998,7 @@
         <v>-79.5</v>
       </c>
       <c r="I84">
-        <v>10.10660980375072</v>
+        <v>10.13617422233814</v>
       </c>
       <c r="J84" t="s">
         <v>509</v>
@@ -52222,7 +52153,7 @@
         <v>-79.5</v>
       </c>
       <c r="I85">
-        <v>6.554111268798902</v>
+        <v>6.555632342273138</v>
       </c>
       <c r="J85" t="s">
         <v>510</v>
@@ -52371,7 +52302,7 @@
         <v>-79.5</v>
       </c>
       <c r="I86">
-        <v>13.83953692232065</v>
+        <v>13.85457768251861</v>
       </c>
       <c r="J86" t="s">
         <v>511</v>
@@ -52535,7 +52466,7 @@
         <v>-79.5</v>
       </c>
       <c r="I87">
-        <v>12.88042719148312</v>
+        <v>12.95811512352232</v>
       </c>
       <c r="J87" t="s">
         <v>512</v>
@@ -52690,7 +52621,7 @@
         <v>-79.5</v>
       </c>
       <c r="I88">
-        <v>15.65324325213099</v>
+        <v>15.74839424412393</v>
       </c>
       <c r="J88" t="s">
         <v>513</v>
@@ -52845,7 +52776,7 @@
         <v>-79.5</v>
       </c>
       <c r="I89">
-        <v>5.581528126792223</v>
+        <v>5.60288920357043</v>
       </c>
       <c r="J89" t="s">
         <v>514</v>
@@ -53000,7 +52931,7 @@
         <v>-79.5</v>
       </c>
       <c r="I90">
-        <v>8.722372121977614</v>
+        <v>8.738816923455527</v>
       </c>
       <c r="J90" t="s">
         <v>515</v>
@@ -53164,7 +53095,7 @@
         <v>-79.5</v>
       </c>
       <c r="I91">
-        <v>9.907117916528399</v>
+        <v>9.974816887861657</v>
       </c>
       <c r="J91" t="s">
         <v>501</v>
@@ -53328,7 +53259,7 @@
         <v>-79.5</v>
       </c>
       <c r="I92">
-        <v>10.49544564703117</v>
+        <v>10.56447986498608</v>
       </c>
       <c r="J92" t="s">
         <v>516</v>
@@ -53527,9 +53458,6 @@
       <c r="W93">
         <v>27.8859865470852</v>
       </c>
-      <c r="X93">
-        <v>1</v>
-      </c>
       <c r="Y93">
         <v>1</v>
       </c>
@@ -53688,9 +53616,6 @@
       <c r="W94">
         <v>27.8859865470852</v>
       </c>
-      <c r="X94">
-        <v>1</v>
-      </c>
       <c r="Y94">
         <v>1</v>
       </c>
@@ -53808,7 +53733,7 @@
         <v>-94.25</v>
       </c>
       <c r="I95">
-        <v>6.650027499973381</v>
+        <v>6.676535156145438</v>
       </c>
       <c r="J95" t="s">
         <v>517</v>
@@ -53945,7 +53870,7 @@
         <v>-94.25</v>
       </c>
       <c r="I96">
-        <v>9.8433707054606</v>
+        <v>9.882607338126476</v>
       </c>
       <c r="J96" t="s">
         <v>517</v>
@@ -54853,9 +54778,6 @@
       <c r="W102">
         <v>14</v>
       </c>
-      <c r="X102">
-        <v>1</v>
-      </c>
       <c r="Y102">
         <v>1</v>
       </c>
@@ -55008,9 +54930,6 @@
       <c r="W103">
         <v>14</v>
       </c>
-      <c r="X103">
-        <v>1</v>
-      </c>
       <c r="Y103">
         <v>1</v>
       </c>
@@ -62364,7 +62283,7 @@
         <v>-118.563032</v>
       </c>
       <c r="I152">
-        <v>7.42057074354461</v>
+        <v>7.421962128396872</v>
       </c>
       <c r="J152" t="s">
         <v>487</v>
@@ -62531,7 +62450,7 @@
         <v>-118.563032</v>
       </c>
       <c r="I153">
-        <v>6.856465370426228</v>
+        <v>6.855594399494972</v>
       </c>
       <c r="J153" t="s">
         <v>490</v>
@@ -62686,7 +62605,7 @@
         <v>-118.563032</v>
       </c>
       <c r="I154">
-        <v>8.14343690275129</v>
+        <v>8.142589499733068</v>
       </c>
       <c r="J154" t="s">
         <v>487</v>
@@ -62853,7 +62772,7 @@
         <v>-118.563032</v>
       </c>
       <c r="I155">
-        <v>7.368423411851344</v>
+        <v>7.366325302357527</v>
       </c>
       <c r="J155" t="s">
         <v>490</v>
@@ -68671,9 +68590,6 @@
       <c r="W192">
         <v>10.35282258064516</v>
       </c>
-      <c r="X192">
-        <v>1</v>
-      </c>
       <c r="Y192">
         <v>1</v>
       </c>
@@ -68823,9 +68739,6 @@
       <c r="W193">
         <v>10.35282258064516</v>
       </c>
-      <c r="X193">
-        <v>1</v>
-      </c>
       <c r="Y193">
         <v>1</v>
       </c>
@@ -69285,9 +69198,6 @@
       <c r="W196">
         <v>48.51063829787234</v>
       </c>
-      <c r="X196">
-        <v>1</v>
-      </c>
       <c r="Y196">
         <v>1</v>
       </c>
@@ -69437,9 +69347,6 @@
       <c r="W197">
         <v>62.85082872928177</v>
       </c>
-      <c r="X197">
-        <v>1</v>
-      </c>
       <c r="Y197">
         <v>1</v>
       </c>
@@ -69586,9 +69493,6 @@
       <c r="W198">
         <v>50.51194539249146</v>
       </c>
-      <c r="X198">
-        <v>1</v>
-      </c>
       <c r="Y198">
         <v>1</v>
       </c>
@@ -69738,9 +69642,6 @@
       <c r="W199">
         <v>54.79775280898876</v>
       </c>
-      <c r="X199">
-        <v>1</v>
-      </c>
       <c r="Y199">
         <v>1</v>
       </c>
@@ -69902,9 +69803,6 @@
       <c r="W200">
         <v>48.51063829787234</v>
       </c>
-      <c r="X200">
-        <v>1</v>
-      </c>
       <c r="Y200">
         <v>1</v>
       </c>
@@ -70054,9 +69952,6 @@
       <c r="W201">
         <v>62.85082872928177</v>
       </c>
-      <c r="X201">
-        <v>1</v>
-      </c>
       <c r="Y201">
         <v>1</v>
       </c>
@@ -70203,9 +70098,6 @@
       <c r="W202">
         <v>50.51194539249146</v>
       </c>
-      <c r="X202">
-        <v>1</v>
-      </c>
       <c r="Y202">
         <v>1</v>
       </c>
@@ -70355,9 +70247,6 @@
       <c r="W203">
         <v>54.79775280898876</v>
       </c>
-      <c r="X203">
-        <v>1</v>
-      </c>
       <c r="Y203">
         <v>1</v>
       </c>
@@ -82847,9 +82736,6 @@
       <c r="V284" t="b">
         <v>0</v>
       </c>
-      <c r="X284">
-        <v>1</v>
-      </c>
       <c r="Y284">
         <v>0</v>
       </c>
@@ -82906,9 +82792,6 @@
       <c r="V285" t="b">
         <v>0</v>
       </c>
-      <c r="X285">
-        <v>1</v>
-      </c>
       <c r="Y285">
         <v>1</v>
       </c>
@@ -82974,9 +82857,6 @@
       <c r="V286" t="b">
         <v>0</v>
       </c>
-      <c r="X286">
-        <v>1</v>
-      </c>
       <c r="Y286">
         <v>1</v>
       </c>
@@ -83027,9 +82907,6 @@
       <c r="V287" t="b">
         <v>0</v>
       </c>
-      <c r="X287">
-        <v>1</v>
-      </c>
       <c r="Y287">
         <v>1</v>
       </c>
@@ -83089,9 +82966,6 @@
       <c r="V288" t="b">
         <v>0</v>
       </c>
-      <c r="X288">
-        <v>1</v>
-      </c>
       <c r="Y288">
         <v>1</v>
       </c>
@@ -83142,9 +83016,6 @@
       <c r="V289" t="b">
         <v>0</v>
       </c>
-      <c r="X289">
-        <v>1</v>
-      </c>
       <c r="Y289">
         <v>0</v>
       </c>
@@ -83198,9 +83069,6 @@
       <c r="V290" t="b">
         <v>0</v>
       </c>
-      <c r="X290">
-        <v>1</v>
-      </c>
       <c r="Y290">
         <v>0</v>
       </c>
@@ -83266,9 +83134,6 @@
       <c r="V291" t="b">
         <v>0</v>
       </c>
-      <c r="X291">
-        <v>1</v>
-      </c>
       <c r="Y291">
         <v>0</v>
       </c>
@@ -83319,9 +83184,6 @@
       <c r="V292" t="b">
         <v>0</v>
       </c>
-      <c r="X292">
-        <v>1</v>
-      </c>
       <c r="Y292">
         <v>0</v>
       </c>
@@ -83378,9 +83240,6 @@
       <c r="V293" t="b">
         <v>0</v>
       </c>
-      <c r="X293">
-        <v>1</v>
-      </c>
       <c r="Y293">
         <v>1</v>
       </c>
@@ -83446,9 +83305,6 @@
       <c r="V294" t="b">
         <v>0</v>
       </c>
-      <c r="X294">
-        <v>1</v>
-      </c>
       <c r="Y294">
         <v>1</v>
       </c>
@@ -83499,9 +83355,6 @@
       <c r="V295" t="b">
         <v>0</v>
       </c>
-      <c r="X295">
-        <v>1</v>
-      </c>
       <c r="Y295">
         <v>1</v>
       </c>
@@ -83561,9 +83414,6 @@
       <c r="V296" t="b">
         <v>0</v>
       </c>
-      <c r="X296">
-        <v>1</v>
-      </c>
       <c r="Y296">
         <v>1</v>
       </c>
@@ -83614,9 +83464,6 @@
       <c r="V297" t="b">
         <v>0</v>
       </c>
-      <c r="X297">
-        <v>1</v>
-      </c>
       <c r="Y297">
         <v>0</v>
       </c>
@@ -83670,9 +83517,6 @@
       <c r="V298" t="b">
         <v>0</v>
       </c>
-      <c r="X298">
-        <v>1</v>
-      </c>
       <c r="Y298">
         <v>0</v>
       </c>
@@ -83738,9 +83582,6 @@
       <c r="V299" t="b">
         <v>0</v>
       </c>
-      <c r="X299">
-        <v>1</v>
-      </c>
       <c r="Y299">
         <v>0</v>
       </c>
@@ -83821,9 +83662,6 @@
       <c r="V300" t="b">
         <v>0</v>
       </c>
-      <c r="X300">
-        <v>1</v>
-      </c>
       <c r="Y300">
         <v>0</v>
       </c>
@@ -83964,9 +83802,6 @@
       <c r="V301" t="b">
         <v>0</v>
       </c>
-      <c r="X301">
-        <v>1</v>
-      </c>
       <c r="Y301">
         <v>0</v>
       </c>
@@ -84119,9 +83954,6 @@
       <c r="V302" t="b">
         <v>0</v>
       </c>
-      <c r="X302">
-        <v>1</v>
-      </c>
       <c r="Y302">
         <v>0</v>
       </c>
@@ -84262,9 +84094,6 @@
       <c r="V303" t="b">
         <v>0</v>
       </c>
-      <c r="X303">
-        <v>1</v>
-      </c>
       <c r="Y303">
         <v>0</v>
       </c>
@@ -86572,9 +86401,6 @@
       <c r="W318">
         <v>29.43243243243243</v>
       </c>
-      <c r="X318">
-        <v>1</v>
-      </c>
       <c r="Y318">
         <v>1</v>
       </c>
@@ -86739,9 +86565,6 @@
       <c r="W319">
         <v>29.43243243243243</v>
       </c>
-      <c r="X319">
-        <v>1</v>
-      </c>
       <c r="Y319">
         <v>1</v>
       </c>
@@ -87362,9 +87185,6 @@
       <c r="W326">
         <v>54.21637426900586</v>
       </c>
-      <c r="X326">
-        <v>1</v>
-      </c>
       <c r="Y326">
         <v>0</v>
       </c>
@@ -87514,9 +87334,6 @@
       <c r="W327">
         <v>35.33333333333334</v>
       </c>
-      <c r="X327">
-        <v>1</v>
-      </c>
       <c r="Y327">
         <v>0</v>
       </c>
@@ -87666,9 +87483,6 @@
       <c r="W328">
         <v>54.21637426900586</v>
       </c>
-      <c r="X328">
-        <v>1</v>
-      </c>
       <c r="Y328">
         <v>0</v>
       </c>
@@ -87817,9 +87631,6 @@
       </c>
       <c r="W329">
         <v>35.33333333333334</v>
-      </c>
-      <c r="X329">
-        <v>1</v>
       </c>
       <c r="Y329">
         <v>0</v>

</xml_diff>